<commit_message>
Fixed Fe3fet typos, clarified some examples
</commit_message>
<xml_diff>
--- a/docs/Examples/Liquid_Ol_Liq_Themometry/Liquid_only_Thermometry.xlsx
+++ b/docs/Examples/Liquid_Ol_Liq_Themometry/Liquid_only_Thermometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Liquid_Ol_Liq_Themometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C66C528-2111-4169-A6F5-DD77572EF157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F3B4CF-FE2E-4069-BA78-A772E204409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{81A2371C-1752-7741-8A48-BEC2C378A224}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{81A2371C-1752-7741-8A48-BEC2C378A224}"/>
   </bookViews>
   <sheets>
     <sheet name="Liquid_only" sheetId="4" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>H2O_Liq</t>
   </si>
   <si>
-    <t>Fe3FeT_Liq</t>
-  </si>
-  <si>
     <t>SiO2_Ol</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>You can add any other columns you may want, like latitude</t>
+  </si>
+  <si>
+    <t>Fe3Fet_Liq</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93241BA4-AD6A-476B-89F9-77C94F1FACB0}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:AD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -731,24 +731,24 @@
         <v>12</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2">
         <v>57.023601531982401</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="3" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2">
         <v>57.658599853515597</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2">
         <v>60.731201171875</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="5" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2">
         <v>61.532798767089801</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="6" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>52.969100952148402</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2">
         <v>54.050201416015597</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2">
         <v>55.656299591064403</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2">
         <v>49.054698944091797</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2">
         <v>50.625099182128899</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2">
         <v>51.4033012390137</v>
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576FE275-AE04-4DCC-8479-513FB2E844AE}">
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1354,57 +1354,57 @@
         <v>12</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2">
         <v>57.023601531982401</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="3" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2">
         <v>57.658599853515597</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="4" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2">
         <v>60.731201171875</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="5" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2">
         <v>61.532798767089801</v>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="6" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>52.969100952148402</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="7" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2">
         <v>54.050201416015597</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="8" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2">
         <v>55.656299591064403</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="9" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2">
         <v>49.054698944091797</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="10" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2">
         <v>50.625099182128899</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="11" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2">
         <v>51.4033012390137</v>

</xml_diff>